<commit_message>
fix: rename item ids back to original
</commit_message>
<xml_diff>
--- a/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
+++ b/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB514197\Repos\DECAT_Space2Stats\space2stats_api\src\space2stats_ingest\METADATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F099342D-4158-446C-B4BE-1127804A4FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B8E50E-4D3D-47E4-A040-B9B5A32FCC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature Catalog" sheetId="4" r:id="rId1"/>
@@ -1088,19 +1088,19 @@
     <t>Item</t>
   </si>
   <si>
-    <t>nighttime-lights-2013</t>
-  </si>
-  <si>
-    <t>population-2020</t>
-  </si>
-  <si>
-    <t>flood-exposure-15cm-1in100</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
     <t>Climate</t>
+  </si>
+  <si>
+    <t>space2stats_population_2020</t>
+  </si>
+  <si>
+    <t>nighttime_lights_2013</t>
+  </si>
+  <si>
+    <t>flood_exposure_15cm_1in100</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1189,7 +1189,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1637,8 +1636,8 @@
   </sheetPr>
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,7 +1670,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1682,7 +1681,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1693,7 +1692,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1704,7 +1703,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1715,7 +1714,7 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1726,7 +1725,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1737,7 +1736,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1748,7 +1747,7 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1759,7 +1758,7 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1770,7 +1769,7 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1781,7 +1780,7 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1792,7 +1791,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1803,7 +1802,7 @@
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1814,7 +1813,7 @@
         <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1825,7 +1824,7 @@
         <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1836,7 +1835,7 @@
         <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1847,7 +1846,7 @@
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1858,7 +1857,7 @@
         <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1869,7 +1868,7 @@
         <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1880,7 +1879,7 @@
         <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1891,7 +1890,7 @@
         <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1902,7 +1901,7 @@
         <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1913,7 +1912,7 @@
         <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1924,7 +1923,7 @@
         <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1935,7 +1934,7 @@
         <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1946,7 +1945,7 @@
         <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1957,7 +1956,7 @@
         <v>57</v>
       </c>
       <c r="D28" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1968,7 +1967,7 @@
         <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1979,7 +1978,7 @@
         <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1990,7 +1989,7 @@
         <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2001,7 +2000,7 @@
         <v>65</v>
       </c>
       <c r="D32" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2012,7 +2011,7 @@
         <v>67</v>
       </c>
       <c r="D33" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2023,7 +2022,7 @@
         <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2034,7 +2033,7 @@
         <v>71</v>
       </c>
       <c r="D35" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2045,7 +2044,7 @@
         <v>73</v>
       </c>
       <c r="D36" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2056,7 +2055,7 @@
         <v>75</v>
       </c>
       <c r="D37" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2067,7 +2066,7 @@
         <v>77</v>
       </c>
       <c r="D38" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2078,7 +2077,7 @@
         <v>79</v>
       </c>
       <c r="D39" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2089,7 +2088,7 @@
         <v>81</v>
       </c>
       <c r="D40" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2100,7 +2099,7 @@
         <v>83</v>
       </c>
       <c r="D41" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2111,7 +2110,7 @@
         <v>85</v>
       </c>
       <c r="D42" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2154,7 +2153,7 @@
         <v>95</v>
       </c>
       <c r="D47" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2165,7 +2164,7 @@
         <v>97</v>
       </c>
       <c r="D48" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2176,7 +2175,7 @@
         <v>99</v>
       </c>
       <c r="D49" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2187,7 +2186,7 @@
         <v>101</v>
       </c>
       <c r="D50" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2198,7 +2197,7 @@
         <v>103</v>
       </c>
       <c r="D51" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2209,7 +2208,7 @@
         <v>105</v>
       </c>
       <c r="D52" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2220,7 +2219,7 @@
         <v>107</v>
       </c>
       <c r="D53" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2231,7 +2230,7 @@
         <v>109</v>
       </c>
       <c r="D54" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2242,7 +2241,7 @@
         <v>111</v>
       </c>
       <c r="D55" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2253,7 +2252,7 @@
         <v>113</v>
       </c>
       <c r="D56" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2264,7 +2263,7 @@
         <v>115</v>
       </c>
       <c r="D57" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2275,7 +2274,7 @@
         <v>117</v>
       </c>
       <c r="D58" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2286,7 +2285,7 @@
         <v>119</v>
       </c>
       <c r="D59" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2297,7 +2296,7 @@
         <v>121</v>
       </c>
       <c r="D60" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2308,7 +2307,7 @@
         <v>123</v>
       </c>
       <c r="D61" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2319,7 +2318,7 @@
         <v>125</v>
       </c>
       <c r="D62" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2330,7 +2329,7 @@
         <v>127</v>
       </c>
       <c r="D63" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2341,7 +2340,7 @@
         <v>129</v>
       </c>
       <c r="D64" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2352,7 +2351,7 @@
         <v>131</v>
       </c>
       <c r="D65" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2363,7 +2362,7 @@
         <v>133</v>
       </c>
       <c r="D66" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2374,7 +2373,7 @@
         <v>135</v>
       </c>
       <c r="D67" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2385,7 +2384,7 @@
         <v>137</v>
       </c>
       <c r="D68" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2396,7 +2395,7 @@
         <v>139</v>
       </c>
       <c r="D69" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2407,7 +2406,7 @@
         <v>141</v>
       </c>
       <c r="D70" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2418,7 +2417,7 @@
         <v>143</v>
       </c>
       <c r="D71" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2429,7 +2428,7 @@
         <v>145</v>
       </c>
       <c r="D72" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2440,7 +2439,7 @@
         <v>147</v>
       </c>
       <c r="D73" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2451,7 +2450,7 @@
         <v>149</v>
       </c>
       <c r="D74" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2462,7 +2461,7 @@
         <v>151</v>
       </c>
       <c r="D75" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2473,7 +2472,7 @@
         <v>153</v>
       </c>
       <c r="D76" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2484,7 +2483,7 @@
         <v>155</v>
       </c>
       <c r="D77" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2495,7 +2494,7 @@
         <v>157</v>
       </c>
       <c r="D78" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2506,7 +2505,7 @@
         <v>159</v>
       </c>
       <c r="D79" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2517,7 +2516,7 @@
         <v>161</v>
       </c>
       <c r="D80" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2528,7 +2527,7 @@
         <v>163</v>
       </c>
       <c r="D81" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2539,7 +2538,7 @@
         <v>165</v>
       </c>
       <c r="D82" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2550,7 +2549,7 @@
         <v>167</v>
       </c>
       <c r="D83" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2561,7 +2560,7 @@
         <v>169</v>
       </c>
       <c r="D84" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2572,7 +2571,7 @@
         <v>171</v>
       </c>
       <c r="D85" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2583,7 +2582,7 @@
         <v>173</v>
       </c>
       <c r="D86" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2594,7 +2593,7 @@
         <v>175</v>
       </c>
       <c r="D87" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2605,7 +2604,7 @@
         <v>177</v>
       </c>
       <c r="D88" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2616,7 +2615,7 @@
         <v>179</v>
       </c>
       <c r="D89" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2627,7 +2626,7 @@
         <v>181</v>
       </c>
       <c r="D90" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2638,7 +2637,7 @@
         <v>183</v>
       </c>
       <c r="D91" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2649,7 +2648,7 @@
         <v>185</v>
       </c>
       <c r="D92" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2660,7 +2659,7 @@
         <v>187</v>
       </c>
       <c r="D93" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2671,7 +2670,7 @@
         <v>189</v>
       </c>
       <c r="D94" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2682,7 +2681,7 @@
         <v>343</v>
       </c>
       <c r="D95" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2693,7 +2692,7 @@
         <v>344</v>
       </c>
       <c r="D96" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2704,7 +2703,7 @@
         <v>345</v>
       </c>
       <c r="D97" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -2723,8 +2722,8 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2738,91 +2737,91 @@
     <col min="7" max="7" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="J2" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>212</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -2832,12 +2831,12 @@
         <v>213</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>214</v>
@@ -2864,36 +2863,36 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>353</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2997,7 +2996,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
@@ -3010,7 +3009,7 @@
     <col min="3" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>238</v>
       </c>
@@ -3018,7 +3017,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>241</v>
       </c>
@@ -3026,7 +3025,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3034,7 +3033,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>316</v>
       </c>
@@ -3042,7 +3041,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>318</v>
       </c>
@@ -3050,7 +3049,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>320</v>
       </c>
@@ -3058,7 +3057,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>322</v>
       </c>
@@ -3066,7 +3065,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>324</v>
       </c>
@@ -3074,18 +3073,17 @@
         <v>325</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9"/>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>326</v>
       </c>
       <c r="B10"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>322</v>
       </c>
@@ -3093,7 +3091,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>327</v>
       </c>
@@ -3101,7 +3099,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>329</v>
       </c>
@@ -3109,7 +3107,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>331</v>
       </c>
@@ -3117,7 +3115,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>333</v>
       </c>
@@ -3125,7 +3123,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>335</v>
       </c>
@@ -3133,7 +3131,7 @@
         <v>45526</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>336</v>
       </c>
@@ -3141,7 +3139,7 @@
         <v>45526</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>337</v>
       </c>
@@ -3149,62 +3147,61 @@
         <v>338</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>339</v>
       </c>
       <c r="B19"/>
     </row>
-    <row r="20" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21"/>
     </row>
-    <row r="22" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
     </row>
-    <row r="23" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
     </row>
-    <row r="24" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
     </row>
-    <row r="25" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
     </row>
-    <row r="26" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26"/>
     </row>
-    <row r="27" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27"/>
     </row>
-    <row r="28" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
     </row>

</xml_diff>

<commit_message>
added urbanization to STAC catalog
</commit_message>
<xml_diff>
--- a/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
+++ b/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB514197\Repos\DECAT_Space2Stats\space2stats_api\src\space2stats_ingest\METADATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WBG\Work\Code\DECAT_Space2Stats\space2stats_api\src\space2stats_ingest\METADATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B8E50E-4D3D-47E4-A040-B9B5A32FCC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75951DD-AF03-4EED-B6EC-24A912A59526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="392">
   <si>
     <t>variable</t>
   </si>
@@ -1101,13 +1101,127 @@
   </si>
   <si>
     <t>flood_exposure_15cm_1in100</t>
+  </si>
+  <si>
+    <t>Urbanization</t>
+  </si>
+  <si>
+    <t>Urbanization by population and by area</t>
+  </si>
+  <si>
+    <t>Urbanization is analyzed using the GHS-SMOD dataset, including comparisons with population</t>
+  </si>
+  <si>
+    <t>Global Human Settlement Layer (https://human-settlement.emergency.copernicus.eu/degurbaDefinitions.php)</t>
+  </si>
+  <si>
+    <t>Pesaresi M., Ehrlich D., Ferri S., Florczyk A.J., Freire S., Halkia S., Julea A.M., Kemper T., Soille P. and V. Syrris. Operating procedure for the production of the Global Human Settlement Layer from Landsat data of the epochs 1975, 1990, 2000, and 2014. Publications Office of the European Union, EUR 27741 EN, 2016. doi: 10.2788/253582.</t>
+  </si>
+  <si>
+    <t>Copernicus Emergency Management Service</t>
+  </si>
+  <si>
+    <t>1000m</t>
+  </si>
+  <si>
+    <t>11_POP</t>
+  </si>
+  <si>
+    <t>12_POP</t>
+  </si>
+  <si>
+    <t>13_POP</t>
+  </si>
+  <si>
+    <t>21_POP</t>
+  </si>
+  <si>
+    <t>22_POP</t>
+  </si>
+  <si>
+    <t>23_POP</t>
+  </si>
+  <si>
+    <t>30_POP</t>
+  </si>
+  <si>
+    <t>TOTAL_POP</t>
+  </si>
+  <si>
+    <t>COUNT_11</t>
+  </si>
+  <si>
+    <t>COUNT_12</t>
+  </si>
+  <si>
+    <t>COUNT_13</t>
+  </si>
+  <si>
+    <t>COUNT_21</t>
+  </si>
+  <si>
+    <t>COUNT_22</t>
+  </si>
+  <si>
+    <t>COUNT_23</t>
+  </si>
+  <si>
+    <t>COUNT_30</t>
+  </si>
+  <si>
+    <t>Total population in low density rural areas</t>
+  </si>
+  <si>
+    <t>Total population in very low density areas</t>
+  </si>
+  <si>
+    <t>Total population in rural areas</t>
+  </si>
+  <si>
+    <t>Total population in suburban grid cells</t>
+  </si>
+  <si>
+    <t>Total population in semi-dense urban clusters</t>
+  </si>
+  <si>
+    <t>Total population in dense urban clusters</t>
+  </si>
+  <si>
+    <t>Total population in urban centres</t>
+  </si>
+  <si>
+    <t>Total population based on GHS-Pop population</t>
+  </si>
+  <si>
+    <t>Total number of cells in very low density areas</t>
+  </si>
+  <si>
+    <t>Total number of cells in low density rural areas</t>
+  </si>
+  <si>
+    <t>Total number of cells in rural areas</t>
+  </si>
+  <si>
+    <t>Total number of cells in suburban grid cells</t>
+  </si>
+  <si>
+    <t>Total number of cells in semi-dense urban clusters</t>
+  </si>
+  <si>
+    <t>Total number of cells in dense urban clusters</t>
+  </si>
+  <si>
+    <t>Total number of cells in urban centres</t>
+  </si>
+  <si>
+    <t>urbanization_ghssmod</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1131,8 +1245,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1157,6 +1278,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1176,11 +1302,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1201,8 +1328,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1224,7 +1356,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1634,21 +1766,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="H94" sqref="H94"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98:D112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="62.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1662,7 +1794,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1673,7 +1805,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1684,7 +1816,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1695,7 +1827,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1706,7 +1838,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1717,7 +1849,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1728,7 +1860,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1739,7 +1871,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1750,7 +1882,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1761,7 +1893,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1772,7 +1904,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1783,7 +1915,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1794,7 +1926,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1805,7 +1937,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1816,7 +1948,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1827,7 +1959,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1838,7 +1970,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1849,7 +1981,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1860,7 +1992,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1871,7 +2003,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1882,7 +2014,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1893,7 +2025,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1904,7 +2036,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1915,7 +2047,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1926,7 +2058,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1937,7 +2069,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1948,7 +2080,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1959,7 +2091,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1970,7 +2102,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -1981,7 +2113,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -1992,7 +2124,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -2003,7 +2135,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -2014,7 +2146,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>68</v>
       </c>
@@ -2025,7 +2157,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -2036,7 +2168,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -2047,7 +2179,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -2058,7 +2190,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -2069,7 +2201,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -2080,7 +2212,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -2091,7 +2223,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -2102,7 +2234,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -2113,7 +2245,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -2121,7 +2253,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2129,7 +2261,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -2137,7 +2269,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>92</v>
       </c>
@@ -2145,7 +2277,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -2156,7 +2288,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>96</v>
       </c>
@@ -2167,7 +2299,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>98</v>
       </c>
@@ -2178,7 +2310,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -2189,7 +2321,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -2200,7 +2332,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>104</v>
       </c>
@@ -2211,7 +2343,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>106</v>
       </c>
@@ -2222,7 +2354,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>108</v>
       </c>
@@ -2233,7 +2365,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>110</v>
       </c>
@@ -2244,7 +2376,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>112</v>
       </c>
@@ -2255,7 +2387,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>114</v>
       </c>
@@ -2266,7 +2398,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>116</v>
       </c>
@@ -2277,7 +2409,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -2288,7 +2420,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>120</v>
       </c>
@@ -2299,7 +2431,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>122</v>
       </c>
@@ -2310,7 +2442,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>124</v>
       </c>
@@ -2321,7 +2453,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>126</v>
       </c>
@@ -2332,7 +2464,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>128</v>
       </c>
@@ -2343,7 +2475,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>130</v>
       </c>
@@ -2354,7 +2486,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>132</v>
       </c>
@@ -2365,7 +2497,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>134</v>
       </c>
@@ -2376,7 +2508,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>136</v>
       </c>
@@ -2387,7 +2519,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -2398,7 +2530,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>140</v>
       </c>
@@ -2409,7 +2541,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>142</v>
       </c>
@@ -2420,7 +2552,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>144</v>
       </c>
@@ -2431,7 +2563,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>146</v>
       </c>
@@ -2442,7 +2574,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>148</v>
       </c>
@@ -2453,7 +2585,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>150</v>
       </c>
@@ -2464,7 +2596,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>152</v>
       </c>
@@ -2475,7 +2607,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>154</v>
       </c>
@@ -2486,7 +2618,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>156</v>
       </c>
@@ -2497,7 +2629,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>158</v>
       </c>
@@ -2508,7 +2640,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>160</v>
       </c>
@@ -2519,7 +2651,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>162</v>
       </c>
@@ -2530,7 +2662,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>164</v>
       </c>
@@ -2541,7 +2673,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>166</v>
       </c>
@@ -2552,7 +2684,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>168</v>
       </c>
@@ -2563,7 +2695,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>170</v>
       </c>
@@ -2574,7 +2706,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>172</v>
       </c>
@@ -2585,7 +2717,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>174</v>
       </c>
@@ -2596,7 +2728,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>176</v>
       </c>
@@ -2607,7 +2739,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>178</v>
       </c>
@@ -2618,7 +2750,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>180</v>
       </c>
@@ -2629,7 +2761,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>182</v>
       </c>
@@ -2640,7 +2772,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>184</v>
       </c>
@@ -2651,7 +2783,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>186</v>
       </c>
@@ -2662,7 +2794,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>188</v>
       </c>
@@ -2673,7 +2805,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>340</v>
       </c>
@@ -2684,7 +2816,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>341</v>
       </c>
@@ -2695,7 +2827,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>342</v>
       </c>
@@ -2704,6 +2836,171 @@
       </c>
       <c r="D97" t="s">
         <v>353</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>361</v>
+      </c>
+      <c r="B98" t="s">
+        <v>377</v>
+      </c>
+      <c r="D98" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>362</v>
+      </c>
+      <c r="B99" t="s">
+        <v>376</v>
+      </c>
+      <c r="D99" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>363</v>
+      </c>
+      <c r="B100" t="s">
+        <v>378</v>
+      </c>
+      <c r="D100" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>364</v>
+      </c>
+      <c r="B101" t="s">
+        <v>379</v>
+      </c>
+      <c r="D101" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>365</v>
+      </c>
+      <c r="B102" t="s">
+        <v>380</v>
+      </c>
+      <c r="D102" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>366</v>
+      </c>
+      <c r="B103" t="s">
+        <v>381</v>
+      </c>
+      <c r="D103" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>367</v>
+      </c>
+      <c r="B104" t="s">
+        <v>382</v>
+      </c>
+      <c r="D104" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>368</v>
+      </c>
+      <c r="B105" t="s">
+        <v>383</v>
+      </c>
+      <c r="D105" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>369</v>
+      </c>
+      <c r="B106" t="s">
+        <v>384</v>
+      </c>
+      <c r="D106" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>370</v>
+      </c>
+      <c r="B107" t="s">
+        <v>385</v>
+      </c>
+      <c r="D107" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>371</v>
+      </c>
+      <c r="B108" t="s">
+        <v>386</v>
+      </c>
+      <c r="D108" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>372</v>
+      </c>
+      <c r="B109" t="s">
+        <v>387</v>
+      </c>
+      <c r="D109" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>373</v>
+      </c>
+      <c r="B110" t="s">
+        <v>388</v>
+      </c>
+      <c r="D110" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>374</v>
+      </c>
+      <c r="B111" t="s">
+        <v>389</v>
+      </c>
+      <c r="D111" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>375</v>
+      </c>
+      <c r="B112" t="s">
+        <v>390</v>
+      </c>
+      <c r="D112" t="s">
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -2722,25 +3019,25 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="54.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="52.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="54.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>190</v>
       </c>
@@ -2772,7 +3069,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>199</v>
       </c>
@@ -2804,7 +3101,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>207</v>
       </c>
@@ -2834,7 +3131,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>350</v>
       </c>
@@ -2863,7 +3160,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>350</v>
       </c>
@@ -2895,7 +3192,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>225</v>
       </c>
@@ -2924,7 +3221,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>225</v>
       </c>
@@ -2953,35 +3250,66 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="8" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -3002,14 +3330,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>238</v>
       </c>
@@ -3017,7 +3345,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>241</v>
       </c>
@@ -3025,7 +3353,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3033,7 +3361,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>316</v>
       </c>
@@ -3041,7 +3369,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>318</v>
       </c>
@@ -3049,7 +3377,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>320</v>
       </c>
@@ -3057,7 +3385,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>322</v>
       </c>
@@ -3065,7 +3393,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>324</v>
       </c>
@@ -3073,17 +3401,17 @@
         <v>325</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="B9"/>
     </row>
-    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>326</v>
       </c>
       <c r="B10"/>
     </row>
-    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>322</v>
       </c>
@@ -3091,7 +3419,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>327</v>
       </c>
@@ -3099,7 +3427,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>329</v>
       </c>
@@ -3107,7 +3435,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>331</v>
       </c>
@@ -3115,7 +3443,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>333</v>
       </c>
@@ -3123,7 +3451,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>335</v>
       </c>
@@ -3131,7 +3459,7 @@
         <v>45526</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>336</v>
       </c>
@@ -3139,7 +3467,7 @@
         <v>45526</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>337</v>
       </c>
@@ -3147,61 +3475,61 @@
         <v>338</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>339</v>
       </c>
       <c r="B19"/>
     </row>
-    <row r="20" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20"/>
     </row>
-    <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="B21"/>
     </row>
-    <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22"/>
     </row>
-    <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23"/>
     </row>
-    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
     </row>
-    <row r="25" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
     </row>
-    <row r="26" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26"/>
     </row>
-    <row r="27" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27"/>
     </row>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28"/>
       <c r="B28"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32"/>
       <c r="B32"/>
     </row>
@@ -3224,14 +3552,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>237</v>
       </c>
@@ -3242,7 +3570,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>240</v>
       </c>
@@ -3253,7 +3581,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3264,7 +3592,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -3275,7 +3603,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>240</v>
       </c>
@@ -3286,7 +3614,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>240</v>
       </c>
@@ -3297,7 +3625,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>240</v>
       </c>
@@ -3306,7 +3634,7 @@
       </c>
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>240</v>
       </c>
@@ -3317,7 +3645,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>240</v>
       </c>
@@ -3328,7 +3656,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>240</v>
       </c>
@@ -3337,7 +3665,7 @@
       </c>
       <c r="C10"/>
     </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>240</v>
       </c>
@@ -3348,7 +3676,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>240</v>
       </c>
@@ -3357,7 +3685,7 @@
       </c>
       <c r="C12"/>
     </row>
-    <row r="13" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>240</v>
       </c>
@@ -3368,7 +3696,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>240</v>
       </c>
@@ -3379,7 +3707,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>240</v>
       </c>
@@ -3390,7 +3718,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>240</v>
       </c>
@@ -3399,7 +3727,7 @@
       </c>
       <c r="C16"/>
     </row>
-    <row r="17" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>240</v>
       </c>
@@ -3410,7 +3738,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>240</v>
       </c>
@@ -3421,7 +3749,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>240</v>
       </c>
@@ -3432,7 +3760,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>240</v>
       </c>
@@ -3441,7 +3769,7 @@
       </c>
       <c r="C20"/>
     </row>
-    <row r="21" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>240</v>
       </c>
@@ -3452,7 +3780,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>240</v>
       </c>
@@ -3463,7 +3791,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>240</v>
       </c>
@@ -3474,7 +3802,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>278</v>
       </c>
@@ -3485,7 +3813,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>278</v>
       </c>
@@ -3496,7 +3824,7 @@
         <v>179.99999095999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>278</v>
       </c>
@@ -3507,7 +3835,7 @@
         <v>-179.99999561999999</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>278</v>
       </c>
@@ -3518,7 +3846,7 @@
         <v>89.987504549999997</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>278</v>
       </c>
@@ -3529,7 +3857,7 @@
         <v>-89.987504549999997</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>278</v>
       </c>
@@ -3538,7 +3866,7 @@
       </c>
       <c r="C29"/>
     </row>
-    <row r="30" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>278</v>
       </c>
@@ -3549,7 +3877,7 @@
         <v>4326</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>278</v>
       </c>
@@ -3560,7 +3888,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>289</v>
       </c>
@@ -3571,7 +3899,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>289</v>
       </c>
@@ -3582,7 +3910,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>289</v>
       </c>
@@ -3593,7 +3921,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>295</v>
       </c>
@@ -3602,7 +3930,7 @@
       </c>
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>295</v>
       </c>
@@ -3613,7 +3941,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>295</v>
       </c>
@@ -3624,7 +3952,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>295</v>
       </c>
@@ -3635,7 +3963,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>302</v>
       </c>
@@ -3646,7 +3974,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>302</v>
       </c>
@@ -3657,7 +3985,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>302</v>
       </c>
@@ -3668,7 +3996,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>309</v>
       </c>
@@ -3679,7 +4007,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>309</v>
       </c>
@@ -3690,7 +4018,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>309</v>
       </c>
@@ -3701,7 +4029,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>309</v>
       </c>
@@ -3712,11 +4040,11 @@
         <v>314</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46"/>
       <c r="C46"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47"/>
       <c r="C47"/>
     </row>

</xml_diff>

<commit_message>
Adding urbanization to STAC again
</commit_message>
<xml_diff>
--- a/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
+++ b/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WBG\Work\Code\DECAT_Space2Stats\space2stats_api\src\space2stats_ingest\METADATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75951DD-AF03-4EED-B6EC-24A912A59526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16861C5F-261D-4FF4-9657-D0FD76D87B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature Catalog" sheetId="4" r:id="rId1"/>
@@ -1768,7 +1768,7 @@
   </sheetPr>
   <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
       <selection activeCell="D98" sqref="D98:D112"/>
     </sheetView>
   </sheetViews>
@@ -2845,7 +2845,7 @@
       <c r="B98" t="s">
         <v>377</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2856,7 +2856,7 @@
       <c r="B99" t="s">
         <v>376</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2867,7 +2867,7 @@
       <c r="B100" t="s">
         <v>378</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2878,7 +2878,7 @@
       <c r="B101" t="s">
         <v>379</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2889,7 +2889,7 @@
       <c r="B102" t="s">
         <v>380</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2900,7 +2900,7 @@
       <c r="B103" t="s">
         <v>381</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2911,7 +2911,7 @@
       <c r="B104" t="s">
         <v>382</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2922,7 +2922,7 @@
       <c r="B105" t="s">
         <v>383</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2933,7 +2933,7 @@
       <c r="B106" t="s">
         <v>384</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2944,7 +2944,7 @@
       <c r="B107" t="s">
         <v>385</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2955,7 +2955,7 @@
       <c r="B108" t="s">
         <v>386</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2966,7 +2966,7 @@
       <c r="B109" t="s">
         <v>387</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2977,7 +2977,7 @@
       <c r="B110" t="s">
         <v>388</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2988,7 +2988,7 @@
       <c r="B111" t="s">
         <v>389</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2999,7 +2999,7 @@
       <c r="B112" t="s">
         <v>390</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="9" t="s">
         <v>391</v>
       </c>
     </row>
@@ -3019,8 +3019,8 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updating VIIRS data processing and metadata
</commit_message>
<xml_diff>
--- a/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
+++ b/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WBG\Work\Code\DECAT_Space2Stats\space2stats_api\src\space2stats_ingest\METADATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5888E43-BA6B-4027-B8B1-3929AE80742A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5D9324-A887-4DD7-BF34-728E6F79C6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47895" yWindow="-7935" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature Catalog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="356">
   <si>
     <t>Group</t>
   </si>
@@ -1014,6 +1014,100 @@
   </si>
   <si>
     <t>Sum of VIIRS nighttlime lights brightness for 2024</t>
+  </si>
+  <si>
+    <t>Built area</t>
+  </si>
+  <si>
+    <t>Built area (in m2) in 5-year epochs. Source data report built area as total m2 built in 100m pixels at a global scale.</t>
+  </si>
+  <si>
+    <t>Zonal statistics are calculated as simple sum of built area in metres squared.</t>
+  </si>
+  <si>
+    <t>https://human-settlement.emergency.copernicus.eu/datasets.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pesaresi M., Schiavina M., Politis P., Freire S., Krasnodębska K., Uhl J. H., Carioli A., Corbane C., Dijkstra L., Florio P., Friedrich H. K., Gao J., Leyk S., Lu L., Maffenini L., Mari-Rivero I., Melchiorri M., Syrris V., Van Den Hoek J., Kemper T. Advances on the Global Human Settlement Layer by joint assessment of Earth Observation and population survey data, International Journal of Digital Earth 17 (1), 2024 10.1080/17538947.2024.2390454
+</t>
+  </si>
+  <si>
+    <t>100m</t>
+  </si>
+  <si>
+    <t>builtarea_ghsl</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_1985</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_1975</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_1980</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 1975</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 1980</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 1985</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_1990</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 1990</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_1995</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 1995</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_2000</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 2000</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_2005</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 2005</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_2010</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 2010</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_2015</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 2015</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_2020</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 2020</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_2025</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 2025</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_2030</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 2030</t>
   </si>
 </sst>
 </file>
@@ -1507,8 +1601,8 @@
   </sheetPr>
   <dimension ref="A1:D221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2369,57 +2463,153 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D79" s="10"/>
+      <c r="A79" t="s">
+        <v>333</v>
+      </c>
+      <c r="B79" t="s">
+        <v>335</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D80" s="10"/>
-    </row>
-    <row r="81" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D81" s="10"/>
-    </row>
-    <row r="82" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D82" s="10"/>
-    </row>
-    <row r="83" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D83" s="10"/>
-    </row>
-    <row r="84" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D84" s="10"/>
-    </row>
-    <row r="85" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D85" s="10"/>
-    </row>
-    <row r="86" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D86" s="10"/>
-    </row>
-    <row r="87" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D87" s="10"/>
-    </row>
-    <row r="88" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D88" s="10"/>
-    </row>
-    <row r="89" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D89" s="10"/>
-    </row>
-    <row r="90" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D90" s="10"/>
-    </row>
-    <row r="91" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>334</v>
+      </c>
+      <c r="B80" t="s">
+        <v>336</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>332</v>
+      </c>
+      <c r="B81" t="s">
+        <v>337</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>338</v>
+      </c>
+      <c r="B82" t="s">
+        <v>339</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>340</v>
+      </c>
+      <c r="B83" t="s">
+        <v>341</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>342</v>
+      </c>
+      <c r="B84" t="s">
+        <v>343</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>344</v>
+      </c>
+      <c r="B85" t="s">
+        <v>345</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>346</v>
+      </c>
+      <c r="B86" t="s">
+        <v>347</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>348</v>
+      </c>
+      <c r="B87" t="s">
+        <v>349</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>350</v>
+      </c>
+      <c r="B88" t="s">
+        <v>351</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>352</v>
+      </c>
+      <c r="B89" t="s">
+        <v>353</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>354</v>
+      </c>
+      <c r="B90" t="s">
+        <v>355</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D92" s="10"/>
     </row>
-    <row r="93" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D96" s="10"/>
     </row>
     <row r="97" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2814,8 +3004,8 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3080,7 +3270,38 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
     <row r="10" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J11" s="10"/>

</xml_diff>

<commit_message>
add ingest command for climate time series
</commit_message>
<xml_diff>
--- a/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
+++ b/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WBG\Work\Code\DECAT_Space2Stats\space2stats_api\src\space2stats_ingest\METADATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB514197\Repos\DECAT_Space2Stats\space2stats_api\src\space2stats_ingest\METADATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5888E43-BA6B-4027-B8B1-3929AE80742A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B493A5BE-434F-44FD-93FC-0C4C8AA7A54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47895" yWindow="-7935" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="12090" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature Catalog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="331">
   <si>
     <t>Group</t>
   </si>
@@ -797,30 +797,6 @@
     <t>Total population female, 2020</t>
   </si>
   <si>
-    <t>ntl_sum_yyyymm</t>
-  </si>
-  <si>
-    <t>Sum of lights, monthly</t>
-  </si>
-  <si>
-    <t>flood_area_100</t>
-  </si>
-  <si>
-    <t>Area where flood depth is greater than 50 cm, 1-in-100 return period</t>
-  </si>
-  <si>
-    <t>acled_events_yyyy</t>
-  </si>
-  <si>
-    <t>Sum of conflict events in a given year</t>
-  </si>
-  <si>
-    <t>acled_fatalities_yyyy</t>
-  </si>
-  <si>
-    <t>Sum of estimated fatalities from conflict events in a given year</t>
-  </si>
-  <si>
     <t>pop</t>
   </si>
   <si>
@@ -1014,6 +990,48 @@
   </si>
   <si>
     <t>Sum of VIIRS nighttlime lights brightness for 2024</t>
+  </si>
+  <si>
+    <t>Standardized Precipitation Index (SPI)</t>
+  </si>
+  <si>
+    <t>Index for a given timescale measuring drought severity based on precipitation anomalies (SPI) </t>
+  </si>
+  <si>
+    <t>CHIRPS3</t>
+  </si>
+  <si>
+    <t>Climate Hazards Center, World Bank</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>Processed by Benny Instanto (GOST). The SPI was constructed with a 6-month timescale window based on precidipation data from CHIRPS. The resulting index is standardized (-3 to +3) and stored as a netcdf (~5km resolution). The netcdf was converted to h3 using the h3ronpy raster_to_dataframe function which uses the centroid value for each cell.</t>
+  </si>
+  <si>
+    <t>5km</t>
+  </si>
+  <si>
+    <t>spi</t>
+  </si>
+  <si>
+    <t>climate</t>
+  </si>
+  <si>
+    <t>Standardized Precipitation Index (SPI), 6-month timescale</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Month, formatted as YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1164,6 +1182,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1182,8 +1203,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table7" displayName="Table7" ref="A1:D221" totalsRowShown="0">
-  <autoFilter ref="A1:D221" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table7" displayName="Table7" ref="A1:D217" totalsRowShown="0">
+  <autoFilter ref="A1:D217" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="variable"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="description"/>
@@ -1505,21 +1526,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D221"/>
+  <dimension ref="A1:D217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5234375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>165</v>
       </c>
@@ -1533,7 +1554,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>169</v>
       </c>
@@ -1544,7 +1565,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -1555,7 +1576,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -1566,7 +1587,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>176</v>
       </c>
@@ -1577,7 +1598,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>178</v>
       </c>
@@ -1588,7 +1609,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>180</v>
       </c>
@@ -1599,7 +1620,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>182</v>
       </c>
@@ -1610,7 +1631,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>184</v>
       </c>
@@ -1621,7 +1642,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>186</v>
       </c>
@@ -1632,7 +1653,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>188</v>
       </c>
@@ -1643,7 +1664,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>190</v>
       </c>
@@ -1654,7 +1675,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>192</v>
       </c>
@@ -1665,7 +1686,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>194</v>
       </c>
@@ -1676,7 +1697,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>196</v>
       </c>
@@ -1687,7 +1708,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>198</v>
       </c>
@@ -1698,7 +1719,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>200</v>
       </c>
@@ -1709,7 +1730,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>202</v>
       </c>
@@ -1720,7 +1741,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>204</v>
       </c>
@@ -1731,7 +1752,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>206</v>
       </c>
@@ -1742,7 +1763,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>208</v>
       </c>
@@ -1753,7 +1774,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>210</v>
       </c>
@@ -1764,7 +1785,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>212</v>
       </c>
@@ -1775,7 +1796,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>214</v>
       </c>
@@ -1786,7 +1807,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>216</v>
       </c>
@@ -1797,7 +1818,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>218</v>
       </c>
@@ -1808,7 +1829,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>220</v>
       </c>
@@ -1819,7 +1840,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>222</v>
       </c>
@@ -1830,7 +1851,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>224</v>
       </c>
@@ -1841,7 +1862,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>226</v>
       </c>
@@ -1852,7 +1873,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>228</v>
       </c>
@@ -1863,7 +1884,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>230</v>
       </c>
@@ -1874,7 +1895,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>232</v>
       </c>
@@ -1885,7 +1906,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>234</v>
       </c>
@@ -1896,7 +1917,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>236</v>
       </c>
@@ -1907,7 +1928,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>238</v>
       </c>
@@ -1918,7 +1939,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>240</v>
       </c>
@@ -1929,7 +1950,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>242</v>
       </c>
@@ -1940,7 +1961,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>244</v>
       </c>
@@ -1951,7 +1972,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>246</v>
       </c>
@@ -1962,7 +1983,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>248</v>
       </c>
@@ -1973,7 +1994,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>250</v>
       </c>
@@ -1984,818 +2005,802 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>252</v>
       </c>
       <c r="B43" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>254</v>
       </c>
       <c r="B44" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>256</v>
       </c>
       <c r="B45" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
+        <v>274</v>
+      </c>
+      <c r="B46" t="s">
         <v>258</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>275</v>
+      </c>
+      <c r="B47" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="D47" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>276</v>
+      </c>
+      <c r="B48" t="s">
         <v>260</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D48" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>277</v>
+      </c>
+      <c r="B49" t="s">
         <v>261</v>
       </c>
-      <c r="D47" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="D49" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>278</v>
+      </c>
+      <c r="B50" t="s">
         <v>262</v>
-      </c>
-      <c r="B48" t="s">
-        <v>263</v>
-      </c>
-      <c r="D48" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>264</v>
-      </c>
-      <c r="B49" t="s">
-        <v>265</v>
-      </c>
-      <c r="D49" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>282</v>
-      </c>
-      <c r="B50" t="s">
-        <v>266</v>
       </c>
       <c r="D50" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B51" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D51" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B52" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D52" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B53" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D53" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B54" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D54" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B55" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B56" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D56" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B57" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D57" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B58" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D58" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B59" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D59" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B60" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D60" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B61" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D61" s="13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
+        <v>291</v>
+      </c>
+      <c r="B62" t="s">
+        <v>304</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>292</v>
+      </c>
+      <c r="B63" t="s">
+        <v>305</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>293</v>
+      </c>
+      <c r="B64" t="s">
+        <v>306</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
         <v>294</v>
       </c>
-      <c r="B62" t="s">
-        <v>278</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="B65" t="s">
+        <v>307</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
         <v>295</v>
       </c>
-      <c r="B63" t="s">
-        <v>279</v>
-      </c>
-      <c r="D63" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="B66" t="s">
+        <v>308</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
         <v>296</v>
       </c>
-      <c r="B64" t="s">
-        <v>280</v>
-      </c>
-      <c r="D64" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="B67" t="s">
+        <v>309</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
         <v>297</v>
       </c>
-      <c r="B65" t="s">
-        <v>281</v>
-      </c>
-      <c r="D65" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="B68" t="s">
+        <v>310</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>298</v>
+      </c>
+      <c r="B69" t="s">
+        <v>311</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
         <v>299</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B70" t="s">
         <v>312</v>
       </c>
-      <c r="D66" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="D70" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
         <v>300</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B71" t="s">
         <v>313</v>
       </c>
-      <c r="D67" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="D71" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
         <v>301</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B72" t="s">
         <v>314</v>
       </c>
-      <c r="D68" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="D72" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
         <v>302</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B73" t="s">
         <v>315</v>
       </c>
-      <c r="D69" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="D73" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
         <v>303</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B74" t="s">
         <v>316</v>
       </c>
-      <c r="D70" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>304</v>
-      </c>
-      <c r="B71" t="s">
-        <v>317</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>305</v>
-      </c>
-      <c r="B72" t="s">
-        <v>318</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>306</v>
-      </c>
-      <c r="B73" t="s">
-        <v>319</v>
-      </c>
-      <c r="D73" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>307</v>
-      </c>
-      <c r="B74" t="s">
-        <v>320</v>
-      </c>
       <c r="D74" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>308</v>
+        <v>324</v>
       </c>
       <c r="B75" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="B76" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>310</v>
-      </c>
-      <c r="B77" t="s">
-        <v>323</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>311</v>
-      </c>
-      <c r="B78" t="s">
-        <v>324</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D77" s="10"/>
+    </row>
+    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D78" s="10"/>
+    </row>
+    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D80" s="10"/>
     </row>
-    <row r="81" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D81" s="10"/>
     </row>
-    <row r="82" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D82" s="10"/>
     </row>
-    <row r="83" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D84" s="10"/>
     </row>
-    <row r="85" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D85" s="10"/>
     </row>
-    <row r="86" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D86" s="10"/>
     </row>
-    <row r="87" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D87" s="10"/>
     </row>
-    <row r="88" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D88" s="10"/>
     </row>
-    <row r="89" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D90" s="10"/>
     </row>
-    <row r="91" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D92" s="10"/>
     </row>
-    <row r="93" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D101" s="10"/>
     </row>
-    <row r="102" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D107" s="10"/>
     </row>
-    <row r="108" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D115" s="10"/>
     </row>
-    <row r="116" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D116" s="10"/>
     </row>
-    <row r="117" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D118" s="10"/>
     </row>
-    <row r="119" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D120" s="10"/>
     </row>
-    <row r="121" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D135" s="10"/>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D136" s="10"/>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D137" s="10"/>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D138" s="10"/>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D139" s="10"/>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D140" s="10"/>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D141" s="10"/>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D142" s="10"/>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D143" s="10"/>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D144" s="10"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D145" s="10"/>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D146" s="10"/>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D147" s="10"/>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D148" s="10"/>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D149" s="10"/>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D150" s="10"/>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D151" s="10"/>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D152" s="10"/>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D153" s="10"/>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D154" s="10"/>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D155" s="10"/>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D156" s="10"/>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D157" s="10"/>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D158" s="10"/>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D159" s="10"/>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D160" s="10"/>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D161" s="10"/>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D162" s="10"/>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D163" s="10"/>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D164" s="10"/>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D165" s="10"/>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D166" s="10"/>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D167" s="10"/>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D168" s="10"/>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D169" s="10"/>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D170" s="10"/>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D171" s="10"/>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D172" s="10"/>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D173" s="10"/>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D174" s="10"/>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D175" s="10"/>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D176" s="10"/>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D177" s="10"/>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D178" s="10"/>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D179" s="10"/>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D180" s="10"/>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D181" s="10"/>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D182" s="10"/>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D183" s="10"/>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D184" s="10"/>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D185" s="10"/>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D186" s="10"/>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D187" s="10"/>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D188" s="10"/>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D189" s="10"/>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D190" s="10"/>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D191" s="10"/>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D192" s="10"/>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D193" s="10"/>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D194" s="10"/>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D195" s="10"/>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D196" s="10"/>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D197" s="10"/>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D198" s="10"/>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D199" s="10"/>
     </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D200" s="10"/>
     </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D201" s="10"/>
     </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D202" s="10"/>
     </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D203" s="10"/>
     </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D204" s="10"/>
     </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D205" s="10"/>
     </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D206" s="10"/>
     </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D207" s="10"/>
     </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D208" s="10"/>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D209" s="10"/>
     </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D210" s="10"/>
     </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D211" s="10"/>
     </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D212" s="10"/>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D213" s="10"/>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D214" s="10"/>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D215" s="10"/>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D216" s="10"/>
     </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D217" s="10"/>
-    </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D218" s="10"/>
-    </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D219" s="10"/>
-    </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D220" s="10"/>
-    </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D221" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2814,26 +2819,26 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.89453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.1015625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5234375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.1015625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1015625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.68359375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.41796875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="7" t="s">
         <v>105</v>
       </c>
@@ -2864,8 +2869,14 @@
       <c r="J1" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>113</v>
       </c>
@@ -2897,7 +2908,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
         <v>123</v>
       </c>
@@ -2926,10 +2937,10 @@
         <v>130</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="10" t="s">
         <v>131</v>
       </c>
@@ -2958,7 +2969,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="11" t="s">
         <v>131</v>
       </c>
@@ -2990,7 +3001,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="10" t="s">
         <v>145</v>
       </c>
@@ -3019,7 +3030,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
         <v>145</v>
       </c>
@@ -3048,7 +3059,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12" t="s">
         <v>157</v>
       </c>
@@ -3080,40 +3091,78 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="K9" s="14">
+        <v>38353</v>
+      </c>
+      <c r="L9" s="14">
+        <v>45627</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
     </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3124,15 +3173,17 @@
   </sheetPr>
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.5234375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -3140,7 +3191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -3148,7 +3199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>79</v>
       </c>
@@ -3156,7 +3207,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
@@ -3164,7 +3215,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>83</v>
       </c>
@@ -3172,7 +3223,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>85</v>
       </c>
@@ -3180,7 +3231,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>87</v>
       </c>
@@ -3188,7 +3239,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>89</v>
       </c>
@@ -3196,13 +3247,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>87</v>
       </c>
@@ -3210,7 +3261,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>92</v>
       </c>
@@ -3218,7 +3269,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>94</v>
       </c>
@@ -3226,7 +3277,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>96</v>
       </c>
@@ -3234,7 +3285,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
         <v>98</v>
       </c>
@@ -3242,7 +3293,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
         <v>100</v>
       </c>
@@ -3250,7 +3301,7 @@
         <v>45526</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>101</v>
       </c>
@@ -3258,7 +3309,7 @@
         <v>45526</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
         <v>102</v>
       </c>
@@ -3266,24 +3317,24 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="25" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="26" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="27" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="29" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="30" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="31" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="32" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3301,14 +3352,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.68359375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3319,7 +3370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3330,7 +3381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3341,7 +3392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3352,7 +3403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3363,7 +3414,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3374,7 +3425,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3382,7 +3433,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -3393,7 +3444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -3404,7 +3455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -3412,7 +3463,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -3423,7 +3474,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -3431,7 +3482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -3442,7 +3493,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -3453,7 +3504,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -3464,7 +3515,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -3472,7 +3523,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
@@ -3483,7 +3534,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -3494,7 +3545,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -3505,7 +3556,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -3513,7 +3564,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -3524,7 +3575,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -3535,7 +3586,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -3546,7 +3597,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -3557,7 +3608,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -3568,7 +3619,7 @@
         <v>179.99999095999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -3579,7 +3630,7 @@
         <v>-179.99999561999999</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -3590,7 +3641,7 @@
         <v>89.987504549999997</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -3601,7 +3652,7 @@
         <v>-89.987504549999997</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -3609,7 +3660,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -3620,7 +3671,7 @@
         <v>4326</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -3631,7 +3682,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -3642,7 +3693,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -3653,7 +3704,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -3664,7 +3715,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -3672,7 +3723,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -3683,7 +3734,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -3694,7 +3745,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -3705,7 +3756,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -3716,7 +3767,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -3727,7 +3778,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -3738,7 +3789,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -3749,7 +3800,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>73</v>
       </c>
@@ -3760,7 +3811,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>73</v>
       </c>
@@ -3771,7 +3822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="s">
         <v>73</v>
       </c>
@@ -3782,8 +3833,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="47" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
add ingest command for climate time series (#118)
* add ingest command for climate time series

* rm commented code
</commit_message>
<xml_diff>
--- a/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
+++ b/space2stats_api/src/space2stats_ingest/METADATA/Space2Stats Metadata Content.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WBG\Work\Code\DECAT_Space2Stats\space2stats_api\src\space2stats_ingest\METADATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB514197\Repos\DECAT_Space2Stats\space2stats_api\src\space2stats_ingest\METADATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5D9324-A887-4DD7-BF34-728E6F79C6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77ACBE1F-54BA-4C4A-90D7-1D3F06488675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature Catalog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="362">
   <si>
     <t>Group</t>
   </si>
@@ -797,30 +797,6 @@
     <t>Total population female, 2020</t>
   </si>
   <si>
-    <t>ntl_sum_yyyymm</t>
-  </si>
-  <si>
-    <t>Sum of lights, monthly</t>
-  </si>
-  <si>
-    <t>flood_area_100</t>
-  </si>
-  <si>
-    <t>Area where flood depth is greater than 50 cm, 1-in-100 return period</t>
-  </si>
-  <si>
-    <t>acled_events_yyyy</t>
-  </si>
-  <si>
-    <t>Sum of conflict events in a given year</t>
-  </si>
-  <si>
-    <t>acled_fatalities_yyyy</t>
-  </si>
-  <si>
-    <t>Sum of estimated fatalities from conflict events in a given year</t>
-  </si>
-  <si>
     <t>pop</t>
   </si>
   <si>
@@ -1014,6 +990,48 @@
   </si>
   <si>
     <t>Sum of VIIRS nighttlime lights brightness for 2024</t>
+  </si>
+  <si>
+    <t>Standardized Precipitation Index (SPI)</t>
+  </si>
+  <si>
+    <t>Index for a given timescale measuring drought severity based on precipitation anomalies (SPI) </t>
+  </si>
+  <si>
+    <t>CHIRPS3</t>
+  </si>
+  <si>
+    <t>Climate Hazards Center, World Bank</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>Processed by Benny Instanto (GOST). The SPI was constructed with a 6-month timescale window based on precidipation data from CHIRPS. The resulting index is standardized (-3 to +3) and stored as a netcdf (~5km resolution). The netcdf was converted to h3 using the h3ronpy raster_to_dataframe function which uses the centroid value for each cell.</t>
+  </si>
+  <si>
+    <t>5km</t>
+  </si>
+  <si>
+    <t>spi</t>
+  </si>
+  <si>
+    <t>climate</t>
+  </si>
+  <si>
+    <t>Standardized Precipitation Index (SPI), 6-month timescale</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Month, formatted as YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
   </si>
   <si>
     <t>Built area</t>
@@ -1038,19 +1056,19 @@
     <t>builtarea_ghsl</t>
   </si>
   <si>
+    <t>sum_built_area_m_1975</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 1975</t>
+  </si>
+  <si>
+    <t>sum_built_area_m_1980</t>
+  </si>
+  <si>
+    <t>Total built area (m2) in 1980</t>
+  </si>
+  <si>
     <t>sum_built_area_m_1985</t>
-  </si>
-  <si>
-    <t>sum_built_area_m_1975</t>
-  </si>
-  <si>
-    <t>sum_built_area_m_1980</t>
-  </si>
-  <si>
-    <t>Total built area (m2) in 1975</t>
-  </si>
-  <si>
-    <t>Total built area (m2) in 1980</t>
   </si>
   <si>
     <t>Total built area (m2) in 1985</t>
@@ -1255,8 +1273,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1276,8 +1294,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table7" displayName="Table7" ref="A1:D221" totalsRowShown="0">
-  <autoFilter ref="A1:D221" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table7" displayName="Table7" ref="A1:D217" totalsRowShown="0">
+  <autoFilter ref="A1:D217" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="variable"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="description"/>
@@ -1599,21 +1617,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D221"/>
+  <dimension ref="A1:D217"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5234375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>165</v>
       </c>
@@ -1627,7 +1645,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>169</v>
       </c>
@@ -1638,7 +1656,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -1649,7 +1667,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -1660,7 +1678,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>176</v>
       </c>
@@ -1671,7 +1689,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>178</v>
       </c>
@@ -1682,7 +1700,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>180</v>
       </c>
@@ -1693,7 +1711,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>182</v>
       </c>
@@ -1704,7 +1722,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>184</v>
       </c>
@@ -1715,7 +1733,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>186</v>
       </c>
@@ -1726,7 +1744,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>188</v>
       </c>
@@ -1737,7 +1755,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>190</v>
       </c>
@@ -1748,7 +1766,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>192</v>
       </c>
@@ -1759,7 +1777,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>194</v>
       </c>
@@ -1770,7 +1788,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>196</v>
       </c>
@@ -1781,7 +1799,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>198</v>
       </c>
@@ -1792,7 +1810,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>200</v>
       </c>
@@ -1803,7 +1821,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>202</v>
       </c>
@@ -1814,7 +1832,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>204</v>
       </c>
@@ -1825,7 +1843,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>206</v>
       </c>
@@ -1836,7 +1854,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>208</v>
       </c>
@@ -1847,7 +1865,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>210</v>
       </c>
@@ -1858,7 +1876,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>212</v>
       </c>
@@ -1869,7 +1887,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>214</v>
       </c>
@@ -1880,7 +1898,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>216</v>
       </c>
@@ -1891,7 +1909,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>218</v>
       </c>
@@ -1902,7 +1920,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>220</v>
       </c>
@@ -1913,7 +1931,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>222</v>
       </c>
@@ -1924,7 +1942,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>224</v>
       </c>
@@ -1935,7 +1953,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>226</v>
       </c>
@@ -1946,7 +1964,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>228</v>
       </c>
@@ -1957,7 +1975,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>230</v>
       </c>
@@ -1968,7 +1986,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>232</v>
       </c>
@@ -1979,7 +1997,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>234</v>
       </c>
@@ -1990,7 +2008,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>236</v>
       </c>
@@ -2001,7 +2019,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>238</v>
       </c>
@@ -2012,7 +2030,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>240</v>
       </c>
@@ -2023,7 +2041,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>242</v>
       </c>
@@ -2034,7 +2052,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>244</v>
       </c>
@@ -2045,7 +2063,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>246</v>
       </c>
@@ -2056,7 +2074,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>248</v>
       </c>
@@ -2067,7 +2085,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>250</v>
       </c>
@@ -2078,914 +2096,898 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>252</v>
       </c>
       <c r="B43" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>254</v>
       </c>
       <c r="B44" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>256</v>
       </c>
       <c r="B45" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
+        <v>274</v>
+      </c>
+      <c r="B46" t="s">
         <v>258</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>275</v>
+      </c>
+      <c r="B47" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="D47" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>276</v>
+      </c>
+      <c r="B48" t="s">
         <v>260</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D48" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>277</v>
+      </c>
+      <c r="B49" t="s">
         <v>261</v>
       </c>
-      <c r="D47" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="D49" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>278</v>
+      </c>
+      <c r="B50" t="s">
         <v>262</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D50" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>279</v>
+      </c>
+      <c r="B51" t="s">
         <v>263</v>
       </c>
-      <c r="D48" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="D51" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>280</v>
+      </c>
+      <c r="B52" t="s">
         <v>264</v>
       </c>
-      <c r="B49" t="s">
+      <c r="D52" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>281</v>
+      </c>
+      <c r="B53" t="s">
         <v>265</v>
       </c>
-      <c r="D49" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="D53" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
         <v>282</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B54" t="s">
         <v>266</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D54" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
         <v>283</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B55" t="s">
         <v>267</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D55" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
         <v>284</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B56" t="s">
         <v>268</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D56" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
         <v>285</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B57" t="s">
         <v>269</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D57" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
         <v>286</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B58" t="s">
         <v>270</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D58" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
         <v>287</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B59" t="s">
         <v>271</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D59" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
         <v>288</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B60" t="s">
         <v>272</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D60" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
         <v>289</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B61" t="s">
         <v>273</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D61" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>291</v>
+      </c>
+      <c r="B62" t="s">
+        <v>304</v>
+      </c>
+      <c r="D62" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="B58" t="s">
-        <v>274</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>291</v>
-      </c>
-      <c r="B59" t="s">
-        <v>275</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    </row>
+    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
         <v>292</v>
       </c>
-      <c r="B60" t="s">
-        <v>276</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="B63" t="s">
+        <v>305</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
         <v>293</v>
       </c>
-      <c r="B61" t="s">
-        <v>277</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="B64" t="s">
+        <v>306</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
         <v>294</v>
       </c>
-      <c r="B62" t="s">
-        <v>278</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="B65" t="s">
+        <v>307</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
         <v>295</v>
       </c>
-      <c r="B63" t="s">
-        <v>279</v>
-      </c>
-      <c r="D63" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="B66" t="s">
+        <v>308</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
         <v>296</v>
       </c>
-      <c r="B64" t="s">
-        <v>280</v>
-      </c>
-      <c r="D64" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="B67" t="s">
+        <v>309</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
         <v>297</v>
       </c>
-      <c r="B65" t="s">
-        <v>281</v>
-      </c>
-      <c r="D65" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="B68" t="s">
+        <v>310</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>298</v>
+      </c>
+      <c r="B69" t="s">
+        <v>311</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
         <v>299</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B70" t="s">
         <v>312</v>
       </c>
-      <c r="D66" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="D70" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
         <v>300</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B71" t="s">
         <v>313</v>
       </c>
-      <c r="D67" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="D71" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
         <v>301</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B72" t="s">
         <v>314</v>
       </c>
-      <c r="D68" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="D72" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
         <v>302</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B73" t="s">
         <v>315</v>
       </c>
-      <c r="D69" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="D73" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
         <v>303</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B74" t="s">
         <v>316</v>
       </c>
-      <c r="D70" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>304</v>
-      </c>
-      <c r="B71" t="s">
-        <v>317</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>305</v>
-      </c>
-      <c r="B72" t="s">
-        <v>318</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>306</v>
-      </c>
-      <c r="B73" t="s">
-        <v>319</v>
-      </c>
-      <c r="D73" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>307</v>
-      </c>
-      <c r="B74" t="s">
-        <v>320</v>
-      </c>
       <c r="D74" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>308</v>
+        <v>324</v>
       </c>
       <c r="B75" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="B76" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="B77" t="s">
-        <v>323</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>311</v>
+        <v>340</v>
       </c>
       <c r="B78" t="s">
-        <v>324</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="B79" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="B80" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="B81" t="s">
+        <v>347</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="B82" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="B83" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="B84" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="B85" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="B86" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="B87" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="B88" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>352</v>
-      </c>
-      <c r="B89" t="s">
-        <v>353</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>354</v>
-      </c>
-      <c r="B90" t="s">
-        <v>355</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D89" s="10"/>
+    </row>
+    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D90" s="10"/>
+    </row>
+    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D92" s="10"/>
     </row>
-    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D101" s="10"/>
     </row>
-    <row r="102" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D107" s="10"/>
     </row>
-    <row r="108" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D115" s="10"/>
     </row>
-    <row r="116" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D116" s="10"/>
     </row>
-    <row r="117" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D118" s="10"/>
     </row>
-    <row r="119" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D120" s="10"/>
     </row>
-    <row r="121" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="4:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D135" s="10"/>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D136" s="10"/>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D137" s="10"/>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D138" s="10"/>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D139" s="10"/>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D140" s="10"/>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D141" s="10"/>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D142" s="10"/>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D143" s="10"/>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D144" s="10"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D145" s="10"/>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D146" s="10"/>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D147" s="10"/>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D148" s="10"/>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D149" s="10"/>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D150" s="10"/>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D151" s="10"/>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D152" s="10"/>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D153" s="10"/>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D154" s="10"/>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D155" s="10"/>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D156" s="10"/>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D157" s="10"/>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D158" s="10"/>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D159" s="10"/>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D160" s="10"/>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D161" s="10"/>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D162" s="10"/>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D163" s="10"/>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D164" s="10"/>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D165" s="10"/>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D166" s="10"/>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D167" s="10"/>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D168" s="10"/>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D169" s="10"/>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D170" s="10"/>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D171" s="10"/>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D172" s="10"/>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D173" s="10"/>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D174" s="10"/>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D175" s="10"/>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D176" s="10"/>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D177" s="10"/>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D178" s="10"/>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D179" s="10"/>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D180" s="10"/>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D181" s="10"/>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D182" s="10"/>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D183" s="10"/>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D184" s="10"/>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D185" s="10"/>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D186" s="10"/>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D187" s="10"/>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D188" s="10"/>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D189" s="10"/>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D190" s="10"/>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D191" s="10"/>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D192" s="10"/>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D193" s="10"/>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D194" s="10"/>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D195" s="10"/>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D196" s="10"/>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D197" s="10"/>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D198" s="10"/>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D199" s="10"/>
     </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D200" s="10"/>
     </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D201" s="10"/>
     </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D202" s="10"/>
     </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D203" s="10"/>
     </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D204" s="10"/>
     </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D205" s="10"/>
     </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D206" s="10"/>
     </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D207" s="10"/>
     </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D208" s="10"/>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D209" s="10"/>
     </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D210" s="10"/>
     </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D211" s="10"/>
     </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D212" s="10"/>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D213" s="10"/>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D214" s="10"/>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D215" s="10"/>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D216" s="10"/>
     </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D217" s="10"/>
-    </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D218" s="10"/>
-    </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D219" s="10"/>
-    </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D220" s="10"/>
-    </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D221" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -3004,26 +3006,26 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.89453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.1015625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5234375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.1015625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1015625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.68359375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.41796875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="7" t="s">
         <v>105</v>
       </c>
@@ -3054,8 +3056,14 @@
       <c r="J1" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>113</v>
       </c>
@@ -3087,7 +3095,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
         <v>123</v>
       </c>
@@ -3116,10 +3124,10 @@
         <v>130</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="10" t="s">
         <v>131</v>
       </c>
@@ -3148,7 +3156,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="11" t="s">
         <v>131</v>
       </c>
@@ -3180,7 +3188,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="10" t="s">
         <v>145</v>
       </c>
@@ -3209,7 +3217,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="10" t="s">
         <v>145</v>
       </c>
@@ -3238,7 +3246,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12" t="s">
         <v>157</v>
       </c>
@@ -3270,71 +3278,109 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="K9" s="13">
+        <v>38353</v>
+      </c>
+      <c r="L9" s="13">
+        <v>45627</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="G9" s="12" t="s">
+      <c r="B10" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
     </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3345,15 +3391,17 @@
   </sheetPr>
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.5234375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -3361,7 +3409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -3369,7 +3417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>79</v>
       </c>
@@ -3377,7 +3425,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
@@ -3385,7 +3433,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>83</v>
       </c>
@@ -3393,7 +3441,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>85</v>
       </c>
@@ -3401,7 +3449,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>87</v>
       </c>
@@ -3409,7 +3457,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>89</v>
       </c>
@@ -3417,13 +3465,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>87</v>
       </c>
@@ -3431,7 +3479,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>92</v>
       </c>
@@ -3439,7 +3487,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>94</v>
       </c>
@@ -3447,7 +3495,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>96</v>
       </c>
@@ -3455,7 +3503,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
         <v>98</v>
       </c>
@@ -3463,7 +3511,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
         <v>100</v>
       </c>
@@ -3471,7 +3519,7 @@
         <v>45526</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>101</v>
       </c>
@@ -3479,7 +3527,7 @@
         <v>45526</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
         <v>102</v>
       </c>
@@ -3487,24 +3535,24 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="25" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="26" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="27" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="29" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="30" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="31" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="32" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3522,14 +3570,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.89453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.68359375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3540,7 +3588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3551,7 +3599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3562,7 +3610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3573,7 +3621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3584,7 +3632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3595,7 +3643,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3603,7 +3651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -3614,7 +3662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -3625,7 +3673,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -3633,7 +3681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -3644,7 +3692,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -3652,7 +3700,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -3663,7 +3711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -3674,7 +3722,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -3685,7 +3733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -3693,7 +3741,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
@@ -3704,7 +3752,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -3715,7 +3763,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -3726,7 +3774,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -3734,7 +3782,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -3745,7 +3793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -3756,7 +3804,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -3767,7 +3815,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -3778,7 +3826,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -3789,7 +3837,7 @@
         <v>179.99999095999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -3800,7 +3848,7 @@
         <v>-179.99999561999999</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -3811,7 +3859,7 @@
         <v>89.987504549999997</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -3822,7 +3870,7 @@
         <v>-89.987504549999997</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -3830,7 +3878,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -3841,7 +3889,7 @@
         <v>4326</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -3852,7 +3900,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -3863,7 +3911,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -3874,7 +3922,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -3885,7 +3933,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -3893,7 +3941,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -3904,7 +3952,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -3915,7 +3963,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -3926,7 +3974,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -3937,7 +3985,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -3948,7 +3996,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -3959,7 +4007,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -3970,7 +4018,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>73</v>
       </c>
@@ -3981,7 +4029,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>73</v>
       </c>
@@ -3992,7 +4040,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="s">
         <v>73</v>
       </c>
@@ -4003,8 +4051,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="47" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>